<commit_message>
*lendo planilha excel para preenchimento do FORMS
*tirando um screenshot a cada FORM preenchido
</commit_message>
<xml_diff>
--- a/excel_vagas_seb/vagas_seb.xlsx
+++ b/excel_vagas_seb/vagas_seb.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C145"/>
+  <dimension ref="A1:C142"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -577,7 +577,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Assistente administrativo  - COTA PCD</t>
+          <t>Assistente administrativo  - PCD</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -594,12 +594,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Assistente administrativo  - PCD</t>
+          <t>Assistente/ Analista / Desenvolvedor</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>Rio de Janeiro - RJ</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -611,12 +611,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Assistente/ Analista / Desenvolvedor</t>
+          <t>Assistente de Áudio e Vídeo</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Rio de Janeiro - RJ</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -628,12 +628,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Assistente de Áudio e Vídeo</t>
+          <t>Assistente de Captação</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>São Paulo - SP</t>
+          <t>Curitiba - PR</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -650,7 +650,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Curitiba - PR</t>
+          <t>Belo Horizonte - MG</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -662,12 +662,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Assistente de Captação</t>
+          <t>Assistente de Captação (Exclusiva para PCD) - Curitiba/PR</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Belo Horizonte - MG</t>
+          <t>Curitiba - PR</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -679,12 +679,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Assistente de Captação (Exclusiva para PCD) - Curitiba/PR</t>
+          <t>Assistente de Captação/Vendas</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Curitiba - PR</t>
+          <t>Florianópolis - SC</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -696,12 +696,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Assistente de Captação/Vendas</t>
+          <t>Assistente de Ensino</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Florianópolis - SC</t>
+          <t>Maceió - AL</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -713,12 +713,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Assistente de Ensino</t>
+          <t>Assistente de ensino - Early</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Maceió - AL</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -730,12 +730,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Assistente de ensino - Early</t>
+          <t>Assistente de Ensino Fundamental 1 (Lower School)</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>São Paulo - SP</t>
+          <t>Ribeirão Preto - SP</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -747,7 +747,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Assistente de Ensino Fundamental 1 (Lower School)</t>
+          <t>Assistente de Ensino Fundamental 2 e Ensino Médio (Middle e High School)</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -764,7 +764,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Assistente de Ensino Fundamental 2 e Ensino Médio (Middle e High School)</t>
+          <t>Assistente de Ensino Infantil (Early Years)</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -781,12 +781,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Assistente de Ensino Infantil (Early Years)</t>
+          <t>Assistente de Ensino - Lower</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -798,12 +798,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Assistente de Ensino - Lower</t>
+          <t>Assistente de Polo - Curitiba</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>São Paulo - SP</t>
+          <t>Curitiba - PR</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -815,7 +815,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Assistente de Polo - Curitiba</t>
+          <t>Assistente Financeiro</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -832,7 +832,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Assistente Financeiro</t>
+          <t>Auxiliar de Atendimento</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -849,12 +849,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Auxiliar de Atendimento</t>
+          <t>Auxiliar de Enfermagem</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Curitiba - PR</t>
+          <t>Salvador - BA</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -866,7 +866,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Auxiliar de Enfermagem</t>
+          <t>Auxiliar de Manutenção</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -883,12 +883,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Auxiliar de Manutenção</t>
+          <t>Auxiliar de Serviços Gerais</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Salvador - BA</t>
+          <t>Ribeirão Preto - SP</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -905,7 +905,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Salvador - BA</t>
+          <t>Belo Horizonte - MG</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -939,7 +939,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>Salvador - BA</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -956,7 +956,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Belo Horizonte - MG</t>
+          <t>Ribeirão Preto - SP</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -973,7 +973,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Florianópolis - SC</t>
+          <t>Vitória - ES</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -990,7 +990,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>Florianópolis - SC</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1002,12 +1002,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Auxiliar de Serviços Gerais</t>
+          <t>Auxiliar de Serviços Gerais - Exclusivo para PCD</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Vitória - ES</t>
+          <t>Rio de Janeiro - RJ</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1019,12 +1019,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Auxiliar de Serviços Gerais - Exclusivo para PCD</t>
+          <t>Auxiliar de Serviços Gerais - PCD</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Rio de Janeiro - RJ</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1036,12 +1036,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Auxiliar de Serviços Gerais - PCD</t>
+          <t>Auxiliar de Serviços Gerais PV</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>São Paulo - SP</t>
+          <t>Florianópolis - SC</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1053,12 +1053,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Auxiliar de Serviços Gerais PV</t>
+          <t>Babá</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Florianópolis - SC</t>
+          <t>Vila Velha - ES</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Vila Velha - ES</t>
+          <t>Ribeirão Preto - SP</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1087,7 +1087,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Babá</t>
+          <t>Banco de Talentos - Estagiário de Pedagogia</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1097,31 +1097,31 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Efetivo</t>
+          <t>Estágio</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Banco de Talentos - Estagiário de Pedagogia</t>
+          <t>Banco de Talentos Maceió - Professor(a)</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>Maceió - AL</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Estágio</t>
+          <t>Docente</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Banco de Talentos Maceió - Professor(a)</t>
+          <t>Banco de Talentos Maceió - Professor(a) Bilíngue</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1138,46 +1138,46 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Banco de Talentos Maceió - Professor(a) Bilíngue</t>
+          <t>Consultor Comercial</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Maceió - AL</t>
+          <t>Ribeirão Preto - SP</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Docente</t>
+          <t>Efetivo</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Banco de talentos - Professor Bilíngue</t>
+          <t>Consultor Comercial</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>Curitiba - PR</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Docente</t>
+          <t>Efetivo</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Banco de Talentos - Professor Português (Ensino Fundamental)</t>
+          <t>Consultor Comercial Maple Bear Poços de Caldas</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>Poços de Caldas - MG</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1189,12 +1189,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Consultor Comercial</t>
+          <t>Controlador de acesso</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>Salvador - BA</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1206,12 +1206,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Consultor Comercial</t>
+          <t>Controlador de Acesso</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Curitiba - PR</t>
+          <t>São José dos Campos - SP</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1223,12 +1223,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Consultor Comercial Maple Bear Poços de Caldas</t>
+          <t>Coordenador de Marketing</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Poços de Caldas - MG</t>
+          <t>Ribeirão Preto - SP</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1240,97 +1240,97 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Controlador de acesso</t>
+          <t>Coordenador de Polo - Trabalho Presencial (Pará/Acre/Manaus)</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Salvador - BA</t>
+          <t>Curitiba - PR</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Efetivo</t>
+          <t>Pessoa jurídica</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Controlador de Acesso</t>
+          <t>Coordenador Pedagógico</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>São José dos Campos - SP</t>
+          <t>Belo Horizonte - MG</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Efetivo</t>
+          <t>Banco de talentos</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Coordenador de Marketing</t>
+          <t>Coordenador Pedagógico Bilíngue</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>Brasília - DF</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Efetivo</t>
+          <t>Docente</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Coordenador de Polo - Trabalho Presencial (Pará/Acre/Manaus)</t>
+          <t>Coordenador Pedagógico Bilíngue</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Curitiba - PR</t>
+          <t>Ipatinga - MG</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Pessoa jurídica</t>
+          <t>Efetivo</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Coordenador Pedagógico</t>
+          <t>Counselor (Orientador Educacional)</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Belo Horizonte - MG</t>
+          <t>Ribeirão Preto - SP</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Banco de talentos</t>
+          <t>Efetivo</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Coordenador Pedagógico Bilíngue</t>
+          <t>Curriculum and Assessment Designer</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Ipatinga - MG</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1342,24 +1342,20 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Coordenador Pedagógico Bilíngue</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Brasília - DF</t>
-        </is>
-      </c>
+          <t>Diretor Pedagógico</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Docente</t>
+          <t>Efetivo</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Counselor (Orientador Educacional)</t>
+          <t>English Head Teacher (Middle/High School)</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1369,44 +1365,48 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Efetivo</t>
+          <t>Docente</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Curriculum and Assessment Designer</t>
+          <t>Estagiário</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>São Paulo - SP</t>
+          <t>Ribeirão Preto - SP</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Efetivo</t>
+          <t>Estágio</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Diretor Pedagógico</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr"/>
+          <t>Estagiário After School</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro - RJ</t>
+        </is>
+      </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Efetivo</t>
+          <t>Estágio</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>English Head Teacher (Middle/High School)</t>
+          <t>Estagiário de Pedagogia</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1416,14 +1416,14 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Docente</t>
+          <t>Estágio</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Estagiário</t>
+          <t>Estagiário de Relacionamento com o Cliente</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1440,12 +1440,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Estagiário After School</t>
+          <t>Estagiário Mídias</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Rio de Janeiro - RJ</t>
+          <t>São José dos Campos - SP</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1457,12 +1457,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Estagiário de Pedagogia</t>
+          <t>Estagiário Pedagógico Bilingue</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>Rio de Janeiro - RJ</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1474,12 +1474,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Estagiário de Relacionamento com o Cliente</t>
+          <t>Estagiário Pedagógico Bilíngue</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>Rio de Janeiro - RJ</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1491,7 +1491,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Estagiário Mídias</t>
+          <t>Estagiários 2024</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1508,12 +1508,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Estagiário Pedagógico Bilingue</t>
+          <t>Estágio</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Rio de Janeiro - RJ</t>
+          <t>Ribeirão Preto - SP</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1525,12 +1525,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Estagiário Pedagógico Bilíngue</t>
+          <t>Estágio 1</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Rio de Janeiro - RJ</t>
+          <t>Brasília - DF</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1542,12 +1542,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Estagiários 2024</t>
+          <t>Estágio / Aprendiz</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>São José dos Campos - SP</t>
+          <t>Ribeirão Preto - SP</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1559,24 +1559,24 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Estágio</t>
+          <t>Estágio Bilíngue</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Estágio</t>
+          <t>Banco de talentos</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Estágio 1</t>
+          <t>Estágio Bilíngue - Pedagogia ou Letras</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -1593,12 +1593,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Estágio / Aprendiz</t>
+          <t>Estágio de Biologia</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>Rio de Janeiro - RJ</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1610,29 +1610,29 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Estágio Bilíngue</t>
+          <t>Estágio de Geografia</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>São Paulo - SP</t>
+          <t>Rio de Janeiro - RJ</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Banco de talentos</t>
+          <t>Estágio</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Estágio Bilíngue - Pedagogia ou Letras</t>
+          <t>Estágio em Pedagogia</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Brasília - DF</t>
+          <t>Vitória - ES</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1644,12 +1644,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Estágio de Biologia</t>
+          <t>Estágio Ensino Fundamental Anos Finas e Ensino Médio - Espanhol</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Rio de Janeiro - RJ</t>
+          <t>São José dos Campos - SP</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -1661,12 +1661,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Estágio de Geografia</t>
+          <t>Estágio Pedagogia</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Rio de Janeiro - RJ</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1678,12 +1678,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Estágio em Pedagogia</t>
+          <t>Estágio Pedagogia</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Vitória - ES</t>
+          <t>Ribeirão Preto - SP</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -1695,12 +1695,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Estágio Ensino Fundamental Anos Finas e Ensino Médio - Espanhol</t>
+          <t>Estágio pedagogia bilíngue</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>São José dos Campos - SP</t>
+          <t>Brasília - DF</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -1712,12 +1712,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Estágio Pedagogia</t>
+          <t>Estágio Pedagogia / Educação Física</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1729,29 +1729,29 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Estágio Pedagogia</t>
+          <t>Estágio (Pedagogia e/ou Letras Inglês)</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>São Paulo - SP</t>
+          <t>Vila Velha - ES</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Estágio</t>
+          <t>Efetivo</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Estágio pedagogia bilíngue</t>
+          <t>Estágio Pedagógico</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Brasília - DF</t>
+          <t>Rio de Janeiro - RJ</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -1763,29 +1763,29 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Estágio Pedagogia / Educação Física</t>
+          <t>Estágio pedagógico (banco de talentos) (CÓPIA)</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>São Paulo - SP</t>
+          <t>Brasília - DF</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Estágio</t>
+          <t>Banco de talentos</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Estágio (Pedagogia e/ou Letras Inglês)</t>
+          <t>Gerente de Operações</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Vila Velha - ES</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -1797,46 +1797,46 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Estágio Pedagógico</t>
+          <t>Guidance Counselor - Orientador Educacional</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Rio de Janeiro - RJ</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Estágio</t>
+          <t>Efetivo</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Estágio pedagógico (banco de talentos) (CÓPIA)</t>
+          <t>Humanities Head Teacher (Middle/High School)</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Brasília - DF</t>
+          <t>Ribeirão Preto - SP</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Banco de talentos</t>
+          <t>Docente</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Gerente de Operações</t>
+          <t>Inspetor</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>São Paulo - SP</t>
+          <t>Curitiba - PR</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -1848,12 +1848,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Guidance Counselor - Orientador Educacional</t>
+          <t>Inspetor(a) de Alunos</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>São Paulo - SP</t>
+          <t>Rio de Janeiro - RJ</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -1865,63 +1865,63 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Humanities Head Teacher (Middle/High School)</t>
+          <t>Integrated Design Specialist</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Docente</t>
+          <t>Efetivo</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Inspetor</t>
+          <t>Mathematics Head Teacher (Middle/High School)</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Curitiba - PR</t>
+          <t>Ribeirão Preto - SP</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Efetivo</t>
+          <t>Docente</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Inspetor(a) de Alunos</t>
+          <t>Monitor</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Rio de Janeiro - RJ</t>
+          <t>Ribeirão Preto - SP</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Efetivo</t>
+          <t>Banco de talentos</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Integrated Design Specialist</t>
+          <t>Monitor</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>São Paulo - SP</t>
+          <t>Belo Horizonte - MG</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -1933,24 +1933,24 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Mathematics Head Teacher (Middle/High School)</t>
+          <t>Monitor - Body Movement</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Docente</t>
+          <t>Efetivo</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Monitor</t>
+          <t>Monitor Fundamental 1 (Lower School)</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -1960,19 +1960,19 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Banco de talentos</t>
+          <t>Efetivo</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Monitor</t>
+          <t>Monitor Infantil (Early Years)</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Belo Horizonte - MG</t>
+          <t>Ribeirão Preto - SP</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -1984,7 +1984,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Monitor - Body Movement</t>
+          <t>Monitor pedagógico - Artes</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -2001,12 +2001,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Monitor Fundamental 1 (Lower School)</t>
+          <t>Monitor pedagógico - Lower</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2018,12 +2018,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Monitor Infantil (Early Years)</t>
+          <t>Monitor pedagógico - Música</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2035,29 +2035,29 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Monitor pedagógico - Artes</t>
+          <t>Natural Sciences Head Teacher (Middle/High School)</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>São Paulo - SP</t>
+          <t>Ribeirão Preto - SP</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Efetivo</t>
+          <t>Docente</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Monitor pedagógico - Lower</t>
+          <t>Oportunidade para Pessoa Com Deficiência - PCD</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>São Paulo - SP</t>
+          <t>Belo Horizonte - MG</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -2069,29 +2069,29 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Monitor pedagógico - Música</t>
+          <t>Orientador Educacional</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>São Paulo - SP</t>
+          <t>Belo Horizonte - MG</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Efetivo</t>
+          <t>Banco de talentos</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Natural Sciences Head Teacher (Middle/High School)</t>
+          <t>Pedagógico Bilíngue</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>Cachoeiro de Itapemirim - ES</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2103,34 +2103,34 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Oportunidade para Pessoa Com Deficiência - PCD</t>
+          <t>Pedagógico Bilíngue</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Belo Horizonte - MG</t>
+          <t>São Paulo</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Efetivo</t>
+          <t>Docente</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Orientador Educacional</t>
+          <t>Pedagógico Bilíngue</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Belo Horizonte - MG</t>
+          <t>Duque de Caxias - RJ</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Banco de talentos</t>
+          <t>Docente</t>
         </is>
       </c>
     </row>
@@ -2154,29 +2154,29 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Pedagógico Bilíngue</t>
+          <t>Pessoa Com Deficiência - PCD</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Duque de Caxias - RJ</t>
+          <t>Ribeirão Preto - SP</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Docente</t>
+          <t>Efetivo</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Pedagógico Bilíngue</t>
+          <t>Portuguese Head Teacher (Middle/High School)</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Cachoeiro de Itapemirim - ES</t>
+          <t>Ribeirão Preto - SP</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -2188,12 +2188,12 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Pedagógico Bilíngue</t>
+          <t>Professor(a)</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>Recife - PE</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -2205,63 +2205,63 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Pessoa Com Deficiência - PCD</t>
+          <t>Professora bilíngue</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>Rio de Janeiro - RJ</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Efetivo</t>
+          <t>Docente</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Portuguese Head Teacher (Middle/High School)</t>
+          <t>Professor(a) Ed. Infantil e Fundamental I  - Banco de talentos</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>Brasília - DF</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Docente</t>
+          <t>Banco de talentos</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Professor(a)</t>
+          <t>Professor(a) Ed. Infantil e Fundamental I - Banco de talentos</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Recife - PE</t>
+          <t>Brasília - DF</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Docente</t>
+          <t>Banco de talentos</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Professora bilíngue</t>
+          <t>Professor bilíngue de Ciências Naturais - Middle e High School</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Rio de Janeiro - RJ</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -2273,12 +2273,12 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Professor(a) Ed. Infantil e Fundamental I  - Banco de talentos</t>
+          <t>Professor bilíngue de Matemática - Fundamental II e Ensino Médio</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Brasília - DF</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -2290,24 +2290,24 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Professor(a) Ed. Infantil e Fundamental I - Banco de talentos</t>
+          <t>Professor bilíngue de Português - Middle e High School</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Brasília - DF</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Banco de talentos</t>
+          <t>Docente</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Professor bilíngue de Ciências Naturais - Middle e High School</t>
+          <t>Professor Bilíngue - Early Years</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -2324,75 +2324,75 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Professor bilíngue de Matemática - Fundamental II e Ensino Médio</t>
+          <t>Professor Bilíngue Ed. Infantil e Fundamental I ( cadastro de reserva )</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>São Paulo - SP</t>
+          <t>Brasília - DF</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Banco de talentos</t>
+          <t>Efetivo</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Professor bilíngue de Português - Middle e High School</t>
+          <t>Professor Bilíngue Ed. Infantil e Fundamental I (cadastro de reserva)</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>São Paulo - SP</t>
+          <t>Brasília - DF</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Docente</t>
+          <t>Estágio</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Professor Bilíngue - Early Years</t>
+          <t>Professor Bilíngue Ensino Fundamental II e Ensino Médio (Cadastro de Reserva)</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>São Paulo - SP</t>
+          <t>Brasília - DF</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Docente</t>
+          <t>Estágio</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Professor Bilíngue Ed. Infantil e Fundamental I ( cadastro de reserva )</t>
+          <t>Professor Bilíngue Maple Bear Sinop</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Brasília - DF</t>
+          <t>Sinop - MT</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Efetivo</t>
+          <t>Docente</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Professor Bilíngue Ed. Infantil e Fundamental I (cadastro de reserva)</t>
+          <t>Professor de ciências bilíngue - Fundamental II  - Cadastro de reserva</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -2402,36 +2402,36 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Estágio</t>
+          <t>Efetivo</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Professor Bilíngue Ensino Fundamental II e Ensino Médio (Cadastro de Reserva)</t>
+          <t>Professor de Ciências Sociais para Middle e High School</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Brasília - DF</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Estágio</t>
+          <t>Docente</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Professor Bilíngue Maple Bear Sinop</t>
+          <t>Professor de Educação Infantil Bilíngue</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Sinop - MT</t>
+          <t>Araxá - MG</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -2443,7 +2443,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Professor de ciências bilíngue - Fundamental II  - Cadastro de reserva</t>
+          <t>Professor de Inglês - Fundamental II  - Cadastro de reserva</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -2460,7 +2460,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Professor de Ciências Sociais para Middle e High School</t>
+          <t>Professor de Inglês para Fundamental II e Ensino Médio</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -2470,31 +2470,31 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Docente</t>
+          <t>Banco de talentos</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Professor de Educação Infantil Bilíngue</t>
+          <t>Professor de matemática bilíngue - Fundamental II  - Cadastro de reserva</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Araxá - MG</t>
+          <t>Brasília - DF</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Docente</t>
+          <t>Efetivo</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Professor de Inglês - Fundamental II  - Cadastro de reserva</t>
+          <t>Professor de Português - Fundamental II e Ensino médio - cadastro de reserva</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -2511,7 +2511,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Professor de Inglês para Fundamental II e Ensino Médio</t>
+          <t>Professor Design e Projetos</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -2521,65 +2521,65 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Banco de talentos</t>
+          <t>Docente</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Professor de matemática bilíngue - Fundamental II  - Cadastro de reserva</t>
+          <t>Professor Educação Infantil e Ensino Fundamental I</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Brasília - DF</t>
+          <t>Belo Horizonte - MG</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Efetivo</t>
+          <t>Banco de talentos</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Professor de Português - Fundamental II e Ensino médio - cadastro de reserva</t>
+          <t>Professor Educação Infantil e Ensino Fundamental I</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Brasília - DF</t>
+          <t>Belo Horizonte - MG</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Efetivo</t>
+          <t>Banco de talentos</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Professor Design e Projetos</t>
+          <t>Professor Educação Infantil e Ensino Fundamental I</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>São Paulo - SP</t>
+          <t>Belo Horizonte</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Docente</t>
+          <t>Banco de talentos</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Professor Educação Infantil e Ensino Fundamental I</t>
+          <t>Professor Ensino Fundamental II e Ensino Médio</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -2596,12 +2596,12 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Professor Educação Infantil e Ensino Fundamental I</t>
+          <t>Professor Ensino Fundamental II e Ensino Médio</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Belo Horizonte - MG</t>
+          <t>Belo Horizonte</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -2613,80 +2613,80 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Professor Educação Infantil e Ensino Fundamental I</t>
+          <t>Professor Ensino Fundamental II e Ensino Médio (Cadastro de Reserva)</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Belo Horizonte</t>
+          <t>Brasília - DF</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Banco de talentos</t>
+          <t>Estágio</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Professor Ensino Fundamental II e Ensino Médio</t>
+          <t>Professor Fundamental 1 (Lower School Head Teacher)</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Belo Horizonte - MG</t>
+          <t>Ribeirão Preto - SP</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Banco de talentos</t>
+          <t>Efetivo</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Professor Ensino Fundamental II e Ensino Médio</t>
+          <t>Professor Infantil (Early Years Head Teacher)</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Belo Horizonte</t>
+          <t>Ribeirão Preto - SP</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Banco de talentos</t>
+          <t>Efetivo</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Professor Ensino Fundamental II e Ensino Médio (Cadastro de Reserva)</t>
+          <t>Professor Polivalente Bilíngue - Lower</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Brasília - DF</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Estágio</t>
+          <t>Docente</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Professor Fundamental 1 (Lower School Head Teacher)</t>
+          <t>Recepcionista</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>Belo Horizonte</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -2698,24 +2698,24 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Professor Infantil (Early Years Head Teacher)</t>
+          <t>Recepcionista</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>Belo Horizonte - MG</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Efetivo</t>
+          <t>Banco de talentos</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Professor Polivalente Bilíngue - Lower</t>
+          <t>School Trips Coordinator</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -2725,19 +2725,19 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Docente</t>
+          <t>Efetivo</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Recepcionista</t>
+          <t>Service Learning Coordinator</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Belo Horizonte</t>
+          <t>São Paulo - SP</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -2749,29 +2749,29 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Recepcionista</t>
+          <t>Teaching and Performance Coach (Middle School)</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Belo Horizonte - MG</t>
+          <t>Ribeirão Preto - SP</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Banco de talentos</t>
+          <t>Efetivo</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>School Trips Coordinator</t>
+          <t>Técnico de Informática</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>São Paulo - SP</t>
+          <t>São José do Rio Preto - SP</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -2783,7 +2783,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Service Learning Coordinator</t>
+          <t>Técnico de TI</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -2800,83 +2800,32 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Teaching and Performance Coach (Middle School)</t>
+          <t>Técnico em Informática</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Ribeirão Preto - SP</t>
+          <t>Belo Horizonte - MG</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Efetivo</t>
+          <t>Banco de talentos</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Técnico de Informática</t>
+          <t>Vaga Presencial em Ribeirão Preto/SP - Consultor Comercial</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>São José do Rio Preto - SP</t>
+          <t>Curitiba - PR</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
-        <is>
-          <t>Efetivo</t>
-        </is>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" t="inlineStr">
-        <is>
-          <t>Técnico de TI</t>
-        </is>
-      </c>
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>São Paulo - SP</t>
-        </is>
-      </c>
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>Efetivo</t>
-        </is>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" t="inlineStr">
-        <is>
-          <t>Técnico em Informática</t>
-        </is>
-      </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>Belo Horizonte - MG</t>
-        </is>
-      </c>
-      <c r="C144" t="inlineStr">
-        <is>
-          <t>Banco de talentos</t>
-        </is>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" t="inlineStr">
-        <is>
-          <t>Vaga Presencial em Ribeirão Preto/SP - Consultor Comercial</t>
-        </is>
-      </c>
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>Curitiba - PR</t>
-        </is>
-      </c>
-      <c r="C145" t="inlineStr">
         <is>
           <t>Efetivo</t>
         </is>

</xml_diff>